<commit_message>
added the finishing touches
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gpain/Documents/Work_Dashboards/Alaska/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3CAEB7-6CB4-B042-A696-4C9C545FC1A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23C295C-9E42-B24B-B17C-05856C82CD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40380" yWindow="500" windowWidth="41060" windowHeight="28300" activeTab="1" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -1403,7 +1403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1445,9 +1445,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2503,10 +2500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09851FDF-4334-4E44-81EF-4155DEF57BA3}">
-  <dimension ref="A1:K123"/>
+  <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:XFD79"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5598,26 +5595,46 @@
       </c>
     </row>
     <row r="79" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="2"/>
-      <c r="B79" s="20"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-      <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
-      <c r="J79" s="2"/>
-      <c r="K79" s="2"/>
+      <c r="A79" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D79" s="2">
+        <v>9</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H79" s="2">
+        <v>0</v>
+      </c>
+      <c r="J79" s="2">
+        <v>5</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="80" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D80" s="4">
         <v>10</v>
@@ -5635,21 +5652,21 @@
         <v>0</v>
       </c>
       <c r="J80" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K80" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>38</v>
+        <v>354</v>
       </c>
       <c r="D81" s="2">
         <v>11</v>
@@ -5661,27 +5678,27 @@
         <v>13</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H81" s="2">
         <v>0</v>
       </c>
       <c r="J81" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B82" s="14" t="s">
-        <v>260</v>
+      <c r="B82" s="2" t="s">
+        <v>261</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D82" s="4">
         <v>12</v>
@@ -5709,11 +5726,11 @@
       <c r="A83" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>261</v>
+      <c r="B83" s="14" t="s">
+        <v>262</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D83" s="2">
         <v>13</v>
@@ -5741,11 +5758,11 @@
       <c r="A84" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B84" s="14" t="s">
-        <v>262</v>
+      <c r="B84" s="2" t="s">
+        <v>263</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D84" s="4">
         <v>14</v>
@@ -5774,10 +5791,10 @@
         <v>30</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D85" s="2">
         <v>15</v>
@@ -5806,10 +5823,10 @@
         <v>30</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D86" s="4">
         <v>16</v>
@@ -5837,11 +5854,11 @@
       <c r="A87" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>269</v>
+      <c r="B87" s="14" t="s">
+        <v>266</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D87" s="2">
         <v>17</v>
@@ -5869,11 +5886,11 @@
       <c r="A88" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B88" s="14" t="s">
-        <v>266</v>
+      <c r="B88" s="2" t="s">
+        <v>267</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D88" s="4">
         <v>18</v>
@@ -5901,11 +5918,11 @@
       <c r="A89" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>267</v>
+      <c r="B89" s="14" t="s">
+        <v>270</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>361</v>
+        <v>36</v>
       </c>
       <c r="D89" s="2">
         <v>19</v>
@@ -5934,10 +5951,10 @@
         <v>30</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>36</v>
+        <v>362</v>
       </c>
       <c r="D90" s="4">
         <v>20</v>
@@ -5965,11 +5982,11 @@
       <c r="A91" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B91" s="14" t="s">
-        <v>271</v>
+      <c r="B91" s="2" t="s">
+        <v>272</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D91" s="2">
         <v>21</v>
@@ -5998,10 +6015,10 @@
         <v>30</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D92" s="4">
         <v>22</v>
@@ -6030,10 +6047,10 @@
         <v>30</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D93" s="2">
         <v>23</v>
@@ -6062,10 +6079,10 @@
         <v>30</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D94" s="4">
         <v>24</v>
@@ -6094,10 +6111,10 @@
         <v>30</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>366</v>
+        <v>276</v>
+      </c>
+      <c r="C95" s="17" t="s">
+        <v>367</v>
       </c>
       <c r="D95" s="2">
         <v>25</v>
@@ -6126,10 +6143,10 @@
         <v>30</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="C96" s="17" t="s">
-        <v>367</v>
+        <v>277</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>368</v>
       </c>
       <c r="D96" s="4">
         <v>26</v>
@@ -6158,10 +6175,10 @@
         <v>30</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D97" s="2">
         <v>27</v>
@@ -6190,10 +6207,10 @@
         <v>30</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D98" s="4">
         <v>28</v>
@@ -6222,10 +6239,10 @@
         <v>30</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D99" s="2">
         <v>29</v>
@@ -6254,10 +6271,10 @@
         <v>30</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D100" s="4">
         <v>30</v>
@@ -6286,10 +6303,10 @@
         <v>30</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D101" s="2">
         <v>31</v>
@@ -6318,10 +6335,10 @@
         <v>30</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>373</v>
+        <v>37</v>
       </c>
       <c r="D102" s="4">
         <v>32</v>
@@ -6350,10 +6367,10 @@
         <v>30</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>37</v>
+        <v>374</v>
       </c>
       <c r="D103" s="2">
         <v>33</v>
@@ -6381,11 +6398,11 @@
       <c r="A104" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B104" s="2" t="s">
-        <v>286</v>
+      <c r="B104" s="14" t="s">
+        <v>287</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D104" s="4">
         <v>34</v>
@@ -6414,10 +6431,10 @@
         <v>30</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D105" s="2">
         <v>35</v>
@@ -6446,10 +6463,10 @@
         <v>30</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D106" s="4">
         <v>36</v>
@@ -6477,11 +6494,11 @@
       <c r="A107" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B107" s="14" t="s">
-        <v>289</v>
+      <c r="B107" s="2" t="s">
+        <v>290</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D107" s="2">
         <v>37</v>
@@ -6510,10 +6527,10 @@
         <v>30</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D108" s="4">
         <v>38</v>
@@ -6542,10 +6559,10 @@
         <v>30</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D109" s="2">
         <v>39</v>
@@ -6574,10 +6591,10 @@
         <v>30</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D110" s="4">
         <v>40</v>
@@ -6606,10 +6623,10 @@
         <v>30</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D111" s="2">
         <v>41</v>
@@ -6638,10 +6655,10 @@
         <v>30</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>382</v>
+        <v>96</v>
       </c>
       <c r="D112" s="4">
         <v>42</v>
@@ -6670,10 +6687,10 @@
         <v>30</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>96</v>
+        <v>383</v>
       </c>
       <c r="D113" s="2">
         <v>43</v>
@@ -6702,10 +6719,10 @@
         <v>30</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D114" s="4">
         <v>44</v>
@@ -6733,11 +6750,11 @@
       <c r="A115" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B115" s="2" t="s">
-        <v>297</v>
+      <c r="B115" s="18" t="s">
+        <v>298</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D115" s="2">
         <v>45</v>
@@ -6765,11 +6782,11 @@
       <c r="A116" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B116" s="18" t="s">
-        <v>298</v>
+      <c r="B116" s="2" t="s">
+        <v>299</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D116" s="4">
         <v>46</v>
@@ -6797,11 +6814,11 @@
       <c r="A117" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B117" s="2" t="s">
-        <v>299</v>
+      <c r="B117" s="18" t="s">
+        <v>300</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D117" s="2">
         <v>47</v>
@@ -6826,36 +6843,7 @@
       </c>
     </row>
     <row r="118" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B118" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="D118" s="4">
-        <v>48</v>
-      </c>
-      <c r="E118" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G118" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H118" s="2">
-        <v>0</v>
-      </c>
-      <c r="J118" s="2">
-        <v>0</v>
-      </c>
-      <c r="K118" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A118" s="2"/>
     </row>
     <row r="119" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2"/>
@@ -6868,9 +6856,6 @@
     </row>
     <row r="122" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2"/>
-    </row>
-    <row r="123" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated files and structure
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gpain/Documents/Work_Dashboards/Alaska/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23C295C-9E42-B24B-B17C-05856C82CD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2121E8A6-B1E9-2D44-8B86-57B21F31F1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
+    <workbookView xWindow="30400" yWindow="660" windowWidth="25360" windowHeight="26340" activeTab="1" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{6A2B6172-D835-5049-8FF9-94BEE80D74AE}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{C4B8D36C-6863-5C40-9A4F-6D5A29124E28}">
       <text>
         <r>
           <rPr>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="445">
   <si>
     <t>table_name</t>
   </si>
@@ -1271,12 +1271,180 @@
   <si>
     <t>prgm_url</t>
   </si>
+  <si>
+    <t>Internal training provided for staff and/or board</t>
+  </si>
+  <si>
+    <t>Internal Training</t>
+  </si>
+  <si>
+    <t>External training provided by organization to community</t>
+  </si>
+  <si>
+    <t>External Training</t>
+  </si>
+  <si>
+    <t>Incorporated throughout strategic plan</t>
+  </si>
+  <si>
+    <t>Strategic Plan</t>
+  </si>
+  <si>
+    <t>Mission/vision/values revision</t>
+  </si>
+  <si>
+    <t>Mission/Vision/Values Revision</t>
+  </si>
+  <si>
+    <t>New partnerships</t>
+  </si>
+  <si>
+    <t>New Partnerships</t>
+  </si>
+  <si>
+    <t>Program or curriculum revision</t>
+  </si>
+  <si>
+    <t>Program or Curriculum Revision</t>
+  </si>
+  <si>
+    <t>Staff or board diversification</t>
+  </si>
+  <si>
+    <t>Staff or Board Diversification</t>
+  </si>
+  <si>
+    <t>More inclusive marketing</t>
+  </si>
+  <si>
+    <t>More Inclusive Marketing</t>
+  </si>
+  <si>
+    <t>Formed affinity/identity groups for staff of similar racial identities</t>
+  </si>
+  <si>
+    <t>Formed Groups</t>
+  </si>
+  <si>
+    <t>In planning stages</t>
+  </si>
+  <si>
+    <t>In Planning Stages</t>
+  </si>
+  <si>
+    <t>Do not know/not applicable</t>
+  </si>
+  <si>
+    <t>Do not know</t>
+  </si>
+  <si>
+    <t>Classroom volunteers/presenters</t>
+  </si>
+  <si>
+    <t>Classroom Volunteers/Presenters</t>
+  </si>
+  <si>
+    <t>Curriculum &amp; instructional materials</t>
+  </si>
+  <si>
+    <t>Curriculum &amp; Instructional Materials</t>
+  </si>
+  <si>
+    <t>Direct teaching</t>
+  </si>
+  <si>
+    <t>Direct Teaching</t>
+  </si>
+  <si>
+    <t>Field trips</t>
+  </si>
+  <si>
+    <t>Field Trips</t>
+  </si>
+  <si>
+    <t>Grant funding</t>
+  </si>
+  <si>
+    <t>Grant Funding</t>
+  </si>
+  <si>
+    <t>Internships</t>
+  </si>
+  <si>
+    <t>Materials &amp; supplies</t>
+  </si>
+  <si>
+    <t>Materials &amp; Supplies</t>
+  </si>
+  <si>
+    <t>Professional development/consulting for administrators</t>
+  </si>
+  <si>
+    <t>Professional Development for Admin</t>
+  </si>
+  <si>
+    <t>Professional development/consulting for teachers</t>
+  </si>
+  <si>
+    <t>Professional Development for Teachers</t>
+  </si>
+  <si>
+    <t>Supporting networks (online/in-person)</t>
+  </si>
+  <si>
+    <t>Supporting Networks</t>
+  </si>
+  <si>
+    <t>Events/Symposiums</t>
+  </si>
+  <si>
+    <t>Residential/overnight programs</t>
+  </si>
+  <si>
+    <t>Residential/Overnight Programs</t>
+  </si>
+  <si>
+    <t>Professional Certification</t>
+  </si>
+  <si>
+    <t>Mobility/wheelchair accommodations</t>
+  </si>
+  <si>
+    <t>Deaf/hearing-impaired accommodations</t>
+  </si>
+  <si>
+    <t>Blind/sight-impaired accommodations</t>
+  </si>
+  <si>
+    <t>Special education accommodations</t>
+  </si>
+  <si>
+    <t>Mobility/wheelchair</t>
+  </si>
+  <si>
+    <t>Deaf/hearing-impaired</t>
+  </si>
+  <si>
+    <t>Blind/sight-impaired</t>
+  </si>
+  <si>
+    <t>Special education</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Fall</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1349,6 +1517,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF112337"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1403,7 +1577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1444,6 +1618,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2502,8 +2680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09851FDF-4334-4E44-81EF-4155DEF57BA3}">
   <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J89" sqref="J89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3754,7 +3932,7 @@
         <v>13</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H21" s="2">
         <v>0</v>
@@ -3764,7 +3942,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3816,19 +3994,19 @@
         <v>22</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H23" s="2">
         <v>0</v>
       </c>
       <c r="J23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>13</v>
@@ -4008,10 +4186,10 @@
         <v>28</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>14</v>
@@ -4040,10 +4218,10 @@
         <v>29</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>14</v>
@@ -4072,10 +4250,10 @@
         <v>30</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>14</v>
@@ -4104,10 +4282,10 @@
         <v>31</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>14</v>
@@ -4488,10 +4666,10 @@
         <v>43</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>14</v>
@@ -4520,10 +4698,10 @@
         <v>44</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>14</v>
@@ -4552,10 +4730,10 @@
         <v>45</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>14</v>
@@ -4584,10 +4762,10 @@
         <v>46</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>14</v>
@@ -4616,10 +4794,10 @@
         <v>47</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>14</v>
@@ -4648,10 +4826,10 @@
         <v>48</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>14</v>
@@ -4680,10 +4858,10 @@
         <v>49</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>14</v>
@@ -4712,10 +4890,10 @@
         <v>50</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>14</v>
@@ -4744,10 +4922,10 @@
         <v>51</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>14</v>
@@ -4776,10 +4954,10 @@
         <v>52</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>14</v>
@@ -4808,10 +4986,10 @@
         <v>53</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>14</v>
@@ -4840,10 +5018,10 @@
         <v>54</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>14</v>
@@ -4872,10 +5050,10 @@
         <v>55</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>14</v>
@@ -4904,10 +5082,10 @@
         <v>56</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>14</v>
@@ -4936,10 +5114,10 @@
         <v>57</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>14</v>
@@ -4968,10 +5146,10 @@
         <v>58</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>14</v>
@@ -5000,10 +5178,10 @@
         <v>59</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>14</v>
@@ -5032,10 +5210,10 @@
         <v>60</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>14</v>
@@ -5064,10 +5242,10 @@
         <v>61</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>14</v>
@@ -5096,10 +5274,10 @@
         <v>62</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>14</v>
@@ -5128,10 +5306,10 @@
         <v>63</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>14</v>
@@ -5160,10 +5338,10 @@
         <v>64</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>14</v>
@@ -5192,10 +5370,10 @@
         <v>65</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>14</v>
@@ -5320,7 +5498,7 @@
         <v>69</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>14</v>
@@ -5556,7 +5734,7 @@
         <v>0</v>
       </c>
       <c r="J77" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K77" s="2" t="s">
         <v>13</v>
@@ -5620,7 +5798,7 @@
         <v>0</v>
       </c>
       <c r="J79" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K79" s="2" t="s">
         <v>13</v>
@@ -5652,7 +5830,7 @@
         <v>0</v>
       </c>
       <c r="J80" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K80" s="2" t="s">
         <v>13</v>
@@ -5678,16 +5856,16 @@
         <v>13</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H81" s="2">
         <v>0</v>
       </c>
       <c r="J81" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5934,16 +6112,16 @@
         <v>13</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H89" s="2">
         <v>0</v>
       </c>
       <c r="J89" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6481,7 +6659,10 @@
         <v>14</v>
       </c>
       <c r="H106" s="2">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="J106" s="2">
         <v>0</v>
@@ -6504,10 +6685,10 @@
         <v>37</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G107" s="2" t="s">
         <v>14</v>
@@ -6536,10 +6717,10 @@
         <v>38</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G108" s="2" t="s">
         <v>14</v>
@@ -6568,10 +6749,10 @@
         <v>39</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>14</v>
@@ -6600,10 +6781,10 @@
         <v>40</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G110" s="2" t="s">
         <v>14</v>
@@ -6632,10 +6813,10 @@
         <v>41</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>14</v>
@@ -6664,10 +6845,10 @@
         <v>42</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>14</v>
@@ -6696,10 +6877,10 @@
         <v>43</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G113" s="2" t="s">
         <v>14</v>
@@ -6728,10 +6909,10 @@
         <v>44</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G114" s="2" t="s">
         <v>14</v>
@@ -6760,10 +6941,10 @@
         <v>45</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G115" s="2" t="s">
         <v>14</v>
@@ -6792,10 +6973,10 @@
         <v>46</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G116" s="2" t="s">
         <v>14</v>
@@ -6824,10 +7005,10 @@
         <v>47</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>14</v>
@@ -6865,16 +7046,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1373AD-CAFE-FC46-B12F-4E16ECB9F9F7}">
-  <dimension ref="A1:N94"/>
+  <dimension ref="A1:N139"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView topLeftCell="A105" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" customWidth="1"/>
+    <col min="3" max="3" width="55.5" customWidth="1"/>
     <col min="4" max="4" width="35.1640625" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="19.5" customWidth="1"/>
@@ -8241,16 +8422,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>39</v>
+        <v>212</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>13</v>
+        <v>389</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>13</v>
+        <v>390</v>
       </c>
       <c r="E47" s="2">
         <v>1</v>
@@ -8258,307 +8439,294 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>39</v>
+        <v>212</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>14</v>
+        <v>391</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>14</v>
+        <v>392</v>
       </c>
       <c r="E48" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="E49" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E50" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="E51" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E52" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="E53" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="E54" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E55" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="E56" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E57" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E59" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E60" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B50" s="2" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E61" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B51" s="2" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E62" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B52" s="2" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E63" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B53" s="2" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E64" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B54" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E54" s="2">
-        <v>1</v>
-      </c>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B55" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E55" s="2">
-        <v>2</v>
-      </c>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E56" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B57" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E57" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B58" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E58" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B59" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E59" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E60" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B61" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E61" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B62" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E62" s="2">
-        <v>9</v>
-      </c>
-      <c r="F62" s="16"/>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
-      <c r="N62" s="2"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B63" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E63" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B64" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E64" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>30</v>
       </c>
@@ -8566,16 +8734,18 @@
         <v>264</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="E65" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>30</v>
       </c>
@@ -8583,16 +8753,18 @@
         <v>264</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="E66" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>30</v>
       </c>
@@ -8600,220 +8772,229 @@
         <v>264</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E67" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E68" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E69" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E70" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E71" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E72" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E73" s="2">
+        <v>9</v>
+      </c>
+      <c r="F73" s="16"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+      <c r="M73" s="2"/>
+      <c r="N73" s="2"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E74" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E75" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E76" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E77" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E67" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E68" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B69" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="D69" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="E69" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B70" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C70" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D70" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="E70" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B71" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C71" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="D71" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="E71" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B72" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C72" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="D72" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="E72" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B73" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C73" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="D73" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="E73" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B74" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C74" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="D74" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="E74" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B75" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C75" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="D75" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="E75" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B76" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C76" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="D76" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E76" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B77" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C77" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="D77" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="E77" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B78" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C78" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D78" s="17" t="s">
-        <v>168</v>
-      </c>
       <c r="E78" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B79" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="C79" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="D79" s="17" t="s">
-        <v>170</v>
+      <c r="C79" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E79" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>30</v>
       </c>
@@ -8821,13 +9002,13 @@
         <v>270</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="D80" s="17" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="E80" s="2">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -8838,13 +9019,13 @@
         <v>270</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="E81" s="2">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -8854,14 +9035,14 @@
       <c r="B82" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>175</v>
+      <c r="C82" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="D82" s="17" t="s">
+        <v>154</v>
       </c>
       <c r="E82" s="2">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -8871,14 +9052,14 @@
       <c r="B83" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>176</v>
+      <c r="C83" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D83" s="17" t="s">
+        <v>156</v>
       </c>
       <c r="E83" s="2">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -8888,14 +9069,14 @@
       <c r="B84" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="C84" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>177</v>
+      <c r="C84" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D84" s="17" t="s">
+        <v>158</v>
       </c>
       <c r="E84" s="2">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -8905,14 +9086,14 @@
       <c r="B85" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="C85" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>179</v>
+      <c r="C85" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="D85" s="17" t="s">
+        <v>160</v>
       </c>
       <c r="E85" s="2">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -8920,46 +9101,50 @@
         <v>30</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="C86" t="s">
-        <v>180</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E86" s="2"/>
+        <v>270</v>
+      </c>
+      <c r="C86" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="D86" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="E86" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E87" s="2"/>
+        <v>270</v>
+      </c>
+      <c r="C87" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D87" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E87" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>183</v>
+        <v>270</v>
+      </c>
+      <c r="C88" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D88" s="17" t="s">
+        <v>166</v>
       </c>
       <c r="E88" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -8967,16 +9152,16 @@
         <v>30</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>184</v>
+        <v>270</v>
+      </c>
+      <c r="C89" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D89" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="E89" s="2">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -8984,16 +9169,16 @@
         <v>30</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>185</v>
+        <v>270</v>
+      </c>
+      <c r="C90" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="D90" s="17" t="s">
+        <v>170</v>
       </c>
       <c r="E90" s="2">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -9001,16 +9186,16 @@
         <v>30</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>186</v>
+        <v>270</v>
+      </c>
+      <c r="C91" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D91" s="17" t="s">
+        <v>172</v>
       </c>
       <c r="E91" s="2">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -9018,16 +9203,16 @@
         <v>30</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>187</v>
+        <v>270</v>
+      </c>
+      <c r="C92" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D92" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="E92" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -9035,16 +9220,16 @@
         <v>30</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="E93" s="2">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -9052,17 +9237,639 @@
         <v>30</v>
       </c>
       <c r="B94" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E94" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E95" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B96" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E96" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B97" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C97" t="s">
+        <v>180</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E97" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E98" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B99" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E99" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B100" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C100" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E100" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B101" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E101" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E102" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E103" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B104" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E104" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B105" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="D105" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E94" s="2">
+      <c r="E105" s="2">
         <v>6</v>
       </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B106" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="E106" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B107" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E107" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B108" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E108" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B109" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E109" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B110" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="E110" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B111" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="E111" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B112" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="E112" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B113" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="E113" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D114" t="s">
+        <v>427</v>
+      </c>
+      <c r="E114" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B115" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="E115" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B116" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="E116" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B117" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="E117" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E118" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B119" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="E119" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B120" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C120" s="20" t="s">
+        <v>434</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E120" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B121" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C121" s="20" t="s">
+        <v>435</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="E121" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B122" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C122" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="E122" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B123" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C123" s="20" t="s">
+        <v>437</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="E123" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B124" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C124" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E124" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B125" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="C125" s="20" t="s">
+        <v>442</v>
+      </c>
+      <c r="D125" s="20" t="s">
+        <v>442</v>
+      </c>
+      <c r="E125" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B126" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="C126" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="D126" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="E126" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B127" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="C127" s="20" t="s">
+        <v>443</v>
+      </c>
+      <c r="D127" s="20" t="s">
+        <v>443</v>
+      </c>
+      <c r="E127" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B128" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="C128" s="20" t="s">
+        <v>444</v>
+      </c>
+      <c r="D128" s="20" t="s">
+        <v>444</v>
+      </c>
+      <c r="E128" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="2"/>
+      <c r="B129" s="14"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="2"/>
+      <c r="B130" s="14"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="2"/>
+      <c r="B131" s="14"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="2"/>
+      <c r="B132" s="14"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="2"/>
+      <c r="B133" s="14"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="2"/>
+      <c r="B134" s="14"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="2"/>
+      <c r="B135" s="14"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="2"/>
+      <c r="B136" s="14"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="2"/>
+      <c r="B137" s="14"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="2"/>
+      <c r="B138" s="14"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="2"/>
+      <c r="B139" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed the order of columns
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gpain/Documents/Work_Dashboards/Alaska/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2121E8A6-B1E9-2D44-8B86-57B21F31F1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17B16B8-9B88-AF43-956E-BC7D4C533880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30400" yWindow="660" windowWidth="25360" windowHeight="26340" activeTab="1" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
+    <workbookView xWindow="30400" yWindow="660" windowWidth="35060" windowHeight="26340" activeTab="1" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -1577,7 +1577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1621,9 +1621,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2681,7 +2678,7 @@
   <dimension ref="A1:K122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J89" sqref="J89"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3342,7 +3339,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>13</v>
@@ -3374,7 +3371,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -3406,7 +3403,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>13</v>
@@ -3438,7 +3435,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>13</v>
@@ -3470,7 +3467,7 @@
         <v>197</v>
       </c>
       <c r="D7" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>13</v>
@@ -3502,7 +3499,7 @@
         <v>198</v>
       </c>
       <c r="D8" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>13</v>
@@ -3534,7 +3531,7 @@
         <v>199</v>
       </c>
       <c r="D9" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>13</v>
@@ -3566,7 +3563,7 @@
         <v>200</v>
       </c>
       <c r="D10" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>13</v>
@@ -3598,7 +3595,7 @@
         <v>301</v>
       </c>
       <c r="D11" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>13</v>
@@ -3630,7 +3627,7 @@
         <v>302</v>
       </c>
       <c r="D12" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>13</v>
@@ -3662,7 +3659,7 @@
         <v>19</v>
       </c>
       <c r="D13" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>13</v>
@@ -3694,7 +3691,7 @@
         <v>303</v>
       </c>
       <c r="D14" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>13</v>
@@ -3726,7 +3723,7 @@
         <v>304</v>
       </c>
       <c r="D15" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
@@ -3758,7 +3755,7 @@
         <v>305</v>
       </c>
       <c r="D16" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>13</v>
@@ -3790,7 +3787,7 @@
         <v>306</v>
       </c>
       <c r="D17" s="2">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>13</v>
@@ -9763,7 +9760,7 @@
       <c r="A125" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B125" s="21" t="s">
+      <c r="B125" s="8" t="s">
         <v>289</v>
       </c>
       <c r="C125" s="20" t="s">
@@ -9780,7 +9777,7 @@
       <c r="A126" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B126" s="21" t="s">
+      <c r="B126" s="8" t="s">
         <v>289</v>
       </c>
       <c r="C126" s="20" t="s">
@@ -9797,7 +9794,7 @@
       <c r="A127" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B127" s="21" t="s">
+      <c r="B127" s="8" t="s">
         <v>289</v>
       </c>
       <c r="C127" s="20" t="s">
@@ -9814,7 +9811,7 @@
       <c r="A128" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B128" s="21" t="s">
+      <c r="B128" s="8" t="s">
         <v>289</v>
       </c>
       <c r="C128" s="20" t="s">

</xml_diff>